<commit_message>
ejemplo de k-means en excel
</commit_message>
<xml_diff>
--- a/CAPITULO 3/otros/ejemplo clustering jerarquico.xlsx
+++ b/CAPITULO 3/otros/ejemplo clustering jerarquico.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="29">
   <si>
     <t>sandro</t>
   </si>
@@ -110,6 +110,9 @@
   <si>
     <t>ITERACION 4</t>
   </si>
+  <si>
+    <t>GRUPOS</t>
+  </si>
 </sst>
 </file>
 
@@ -139,15 +142,21 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -183,17 +192,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -207,109 +205,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="49">
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="40">
     <dxf>
       <font>
         <color auto="1"/>
@@ -886,11 +796,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-284587232"/>
-        <c:axId val="-284585056"/>
+        <c:axId val="-369805504"/>
+        <c:axId val="-369802784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-284587232"/>
+        <c:axId val="-369805504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -947,12 +857,12 @@
             <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-284585056"/>
+        <c:crossAx val="-369802784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-284585056"/>
+        <c:axId val="-369802784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1009,7 +919,7 @@
             <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-284587232"/>
+        <c:crossAx val="-369805504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1437,7 +1347,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1533,11 +1442,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-171717632"/>
-        <c:axId val="-171723072"/>
+        <c:axId val="-369808768"/>
+        <c:axId val="-369808224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-171717632"/>
+        <c:axId val="-369808768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1594,12 +1503,12 @@
             <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-171723072"/>
+        <c:crossAx val="-369808224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-171723072"/>
+        <c:axId val="-369808224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1656,7 +1565,7 @@
             <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-171717632"/>
+        <c:crossAx val="-369808768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2346,7 +2255,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2412,11 +2320,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-171716544"/>
-        <c:axId val="-171711104"/>
+        <c:axId val="-369804960"/>
+        <c:axId val="-369806592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-171716544"/>
+        <c:axId val="-369804960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2473,12 +2381,12 @@
             <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-171711104"/>
+        <c:crossAx val="-369806592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-171711104"/>
+        <c:axId val="-369806592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2535,7 +2443,7 @@
             <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-171716544"/>
+        <c:crossAx val="-369804960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3242,7 +3150,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3308,11 +3215,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-171716000"/>
-        <c:axId val="-171715456"/>
+        <c:axId val="-359593216"/>
+        <c:axId val="-359594304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-171716000"/>
+        <c:axId val="-359593216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3369,12 +3276,12 @@
             <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-171715456"/>
+        <c:crossAx val="-359594304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-171715456"/>
+        <c:axId val="-359594304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3431,7 +3338,7 @@
             <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-171716000"/>
+        <c:crossAx val="-359593216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4121,7 +4028,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -4187,11 +4093,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-169941536"/>
-        <c:axId val="-169940448"/>
+        <c:axId val="-359592672"/>
+        <c:axId val="-359596480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-169941536"/>
+        <c:axId val="-359592672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4248,12 +4154,12 @@
             <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-169940448"/>
+        <c:crossAx val="-359596480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-169940448"/>
+        <c:axId val="-359596480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4310,7 +4216,7 @@
             <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-169941536"/>
+        <c:crossAx val="-359592672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5005,7 +4911,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -5071,11 +4976,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-169938272"/>
-        <c:axId val="-169937728"/>
+        <c:axId val="-359595392"/>
+        <c:axId val="-359598656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-169938272"/>
+        <c:axId val="-359595392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5132,12 +5037,12 @@
             <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-169937728"/>
+        <c:crossAx val="-359598656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-169937728"/>
+        <c:axId val="-359598656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5194,7 +5099,7 @@
             <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-169938272"/>
+        <c:crossAx val="-359595392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8752,8 +8657,8 @@
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>414958</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>147431</xdr:rowOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9044,7 +8949,7 @@
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="16" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2:E10"/>
+      <selection pane="bottomLeft" activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9178,85 +9083,93 @@
       </c>
     </row>
     <row r="11" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C11" s="8" t="s">
+      <c r="B11" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="11">
         <v>2</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="11">
         <v>12.5</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C12" s="9" t="s">
+      <c r="B12" s="9"/>
+      <c r="C12" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="11">
         <f>AVERAGE(D3,D8)</f>
         <v>2.5</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="11">
         <f>AVERAGE(E3,E8)</f>
         <v>27.5</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C13" s="9" t="s">
+      <c r="B13" s="9"/>
+      <c r="C13" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="11">
         <f>AVERAGE(D9,D11)</f>
         <v>1</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="11">
         <f>AVERAGE(E9,E11)</f>
         <v>16.25</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C14" s="9" t="s">
+      <c r="B14" s="9"/>
+      <c r="C14" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="11">
         <f>AVERAGE(D12,D13)</f>
         <v>1.75</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="11">
         <f>AVERAGE(E12,E13)</f>
         <v>21.875</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C15" s="9" t="s">
+      <c r="B15" s="9"/>
+      <c r="C15" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="11">
         <f>AVERAGE(D7,D14)</f>
         <v>2.375</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="11">
         <f>AVERAGE(E7,E14)</f>
         <v>30.9375</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C16" s="7" t="s">
+      <c r="B16" s="9"/>
+      <c r="C16" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="11">
         <f>AVERAGE(D10,D15)</f>
         <v>3.1875</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="11">
         <f>AVERAGE(E10,E15)</f>
         <v>15.46875</v>
       </c>
     </row>
     <row r="17" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
     </row>
     <row r="19" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D19" s="4" t="s">
@@ -9994,29 +9907,32 @@
       <c r="E72" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B11:B16"/>
+  </mergeCells>
   <conditionalFormatting sqref="D20:K27">
-    <cfRule type="top10" dxfId="48" priority="5" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="39" priority="5" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31:I37">
-    <cfRule type="top10" dxfId="47" priority="4" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="38" priority="4" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D50:G54">
-    <cfRule type="top10" dxfId="46" priority="7" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="37" priority="7" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D58:F61">
-    <cfRule type="top10" dxfId="45" priority="8" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="36" priority="8" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D65:E67">
-    <cfRule type="top10" dxfId="44" priority="9" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="35" priority="9" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D71:E72">
-    <cfRule type="top10" dxfId="43" priority="10" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="34" priority="10" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D41:H41">
-    <cfRule type="top10" dxfId="42" priority="22" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="33" priority="22" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D42:H46">
-    <cfRule type="top10" dxfId="41" priority="1" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="32" priority="1" bottom="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10028,9 +9944,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K9" sqref="K9"/>
+      <selection pane="bottomLeft" activeCell="O73" sqref="O73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10042,10 +9958,10 @@
     <row r="2" spans="2:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="8" t="s">
         <v>17</v>
       </c>
     </row>
@@ -10200,7 +10116,7 @@
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C17" s="10"/>
+      <c r="C17" s="7"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C18" s="4"/>
@@ -10886,28 +10802,28 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D19:D21">
-    <cfRule type="top10" dxfId="40" priority="32" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="31" priority="32" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19:E21">
-    <cfRule type="top10" dxfId="38" priority="31" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="30" priority="31" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F19:F21">
-    <cfRule type="top10" dxfId="37" priority="30" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="29" priority="30" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G19:G21">
-    <cfRule type="top10" dxfId="36" priority="29" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="28" priority="29" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19:H21">
-    <cfRule type="top10" dxfId="35" priority="28" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="27" priority="28" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I19:I21">
-    <cfRule type="top10" dxfId="34" priority="27" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="26" priority="27" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J19:J21">
-    <cfRule type="top10" dxfId="33" priority="26" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="25" priority="26" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K19:K21">
-    <cfRule type="top10" dxfId="32" priority="25" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="24" priority="25" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D29:D31">
     <cfRule type="top10" dxfId="23" priority="24" bottom="1" rank="1"/>

</xml_diff>